<commit_message>
checklist added and ...
</commit_message>
<xml_diff>
--- a/Skills.xlsx
+++ b/Skills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Learning-List\Learning-List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCC6A3A-E32C-491A-9588-63DBF937BF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8EEC3-C5FC-44A7-80FF-50F86071C77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>All Skills</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Typescript</t>
   </si>
   <si>
-    <t>React.js</t>
-  </si>
-  <si>
     <t>Next.js(App Router)</t>
   </si>
   <si>
@@ -261,13 +258,10 @@
     <t>Next.js(Page router)</t>
   </si>
   <si>
-    <t>React hook form</t>
-  </si>
-  <si>
-    <t>Then projects</t>
-  </si>
-  <si>
     <t>React Hook Form</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -618,442 +612,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="F9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="F11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="F13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="F14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="F15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="F16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>